<commit_message>
saves the figures RSSIxDistance for models
</commit_message>
<xml_diff>
--- a/5-2 GHz Analysis/tables/models_metrics_in_test_set_Geral.xlsx
+++ b/5-2 GHz Analysis/tables/models_metrics_in_test_set_Geral.xlsx
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.770180457870678</v>
+        <v>1.94686351230064</v>
       </c>
       <c r="C6" t="n">
-        <v>6.750750731468653</v>
+        <v>3.291354539467505</v>
       </c>
       <c r="D6" t="n">
-        <v>0.003889305893268413</v>
+        <v>0.7569937851937422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analysis of the models for 5.2 GHz
Analysis of the models for 5.2GHz considering the near, medium, far distances and in general, i.e in the whole dataset.
</commit_message>
<xml_diff>
--- a/5-2 GHz Analysis/tables/models_metrics_in_test_set_Geral.xlsx
+++ b/5-2 GHz Analysis/tables/models_metrics_in_test_set_Geral.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.974201879855123</v>
+        <v>1.955880088503596</v>
       </c>
       <c r="C2" t="n">
-        <v>3.442277665780778</v>
+        <v>3.359480197017807</v>
       </c>
       <c r="D2" t="n">
-        <v>0.7430541532575515</v>
+        <v>0.7524606424109233</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.942103093942143</v>
+        <v>1.977707360461119</v>
       </c>
       <c r="C3" t="n">
-        <v>2.093103448275861</v>
+        <v>3.145172413793103</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7593618510503068</v>
+        <v>0.7412243088690889</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2.205408036062654</v>
+        <v>1.487185414381639</v>
       </c>
       <c r="C4" t="n">
-        <v>3.731318745643458</v>
+        <v>1.709907722195245</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5998423088205515</v>
+        <v>0.9172561303656908</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.968662123782769</v>
+        <v>1.952506025388216</v>
       </c>
       <c r="C5" t="n">
-        <v>3.422145870056096</v>
+        <v>3.338063459239361</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7459260727070747</v>
+        <v>0.7541643351512322</v>
       </c>
     </row>
     <row r="6">

</xml_diff>